<commit_message>
Adding Voleur.java method and implements the test
</commit_message>
<xml_diff>
--- a/cahierDeTests.xlsx
+++ b/cahierDeTests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\donal\Documents\FrontEnd\Citadelles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{299EF204-B532-45B2-9E7F-BCF36728A513}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EF0914B-E39C-4630-8652-0BF3E5000A11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="114">
   <si>
     <t>Le  but de ce cahier de tests est de consigner tous les tests que chaque équipe 
 fait tout au long du projet. Chaque onglet correspondra aux tests de chaque classe du projet.</t>
@@ -371,6 +371,18 @@
   </si>
   <si>
     <t>la chaine de cartère ne peut être vide</t>
+  </si>
+  <si>
+    <t>TestVoleur.test1()</t>
+  </si>
+  <si>
+    <t>TestVoleur.test2()</t>
+  </si>
+  <si>
+    <t>TEST DU VOL D'UN PERSONNAGE</t>
+  </si>
+  <si>
+    <t>Le personnage est bien volé</t>
   </si>
 </sst>
 </file>
@@ -637,7 +649,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -672,8 +684,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2014,8 +2028,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B2:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2528,7 +2542,7 @@
       <c r="F17" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="G17" s="8" t="s">
+      <c r="G17" s="24" t="s">
         <v>53</v>
       </c>
       <c r="H17" s="23">
@@ -2545,28 +2559,68 @@
       </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B18" s="12"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="15"/>
+      <c r="B18" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F18" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="H18" s="23">
+        <v>45233</v>
+      </c>
+      <c r="I18" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="J18" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="K18" s="15" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B19" s="12"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="15"/>
+      <c r="B19" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="E19" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F19" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="H19" s="23">
+        <v>45233</v>
+      </c>
+      <c r="I19" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="J19" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="K19" s="15" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B20" s="12"/>

</xml_diff>

<commit_message>
Adding Eveque.java method and Magicienne.java. implementation and testing
</commit_message>
<xml_diff>
--- a/cahierDeTests.xlsx
+++ b/cahierDeTests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\donal\Documents\FrontEnd\Citadelles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EF0914B-E39C-4630-8652-0BF3E5000A11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7613E09A-F06E-4A50-877E-E46215FB675C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Objectifs" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,10 @@
     <sheet name="test.TestRoi" sheetId="4" r:id="rId4"/>
     <sheet name="test.TestPioche" sheetId="5" r:id="rId5"/>
     <sheet name="test.TestPlateauDeJeu" sheetId="6" r:id="rId6"/>
-    <sheet name="test..." sheetId="7" r:id="rId7"/>
+    <sheet name="test.TestInteraction" sheetId="9" r:id="rId7"/>
+    <sheet name="test.TestAssassin" sheetId="10" r:id="rId8"/>
+    <sheet name="test.TestVoleur" sheetId="11" r:id="rId9"/>
+    <sheet name="test.TestEveque" sheetId="12" r:id="rId10"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
@@ -31,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="116">
   <si>
     <t>Le  but de ce cahier de tests est de consigner tous les tests que chaque équipe 
 fait tout au long du projet. Chaque onglet correspondra aux tests de chaque classe du projet.</t>
@@ -383,6 +386,12 @@
   </si>
   <si>
     <t>Le personnage est bien volé</t>
+  </si>
+  <si>
+    <t>TestEveque.test1()</t>
+  </si>
+  <si>
+    <t>TestEveque.test2()</t>
   </si>
 </sst>
 </file>
@@ -415,7 +424,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -635,13 +644,86 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
+      <left style="medium">
+        <color indexed="64"/>
       </left>
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -649,7 +731,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -684,10 +766,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1107,6 +1199,392 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{191F9536-B5AD-4355-A31F-F84D04ACDB1C}">
+  <dimension ref="B1:K26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="21.5546875" customWidth="1"/>
+    <col min="3" max="3" width="19.77734375" customWidth="1"/>
+    <col min="4" max="4" width="23.88671875" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" customWidth="1"/>
+    <col min="6" max="6" width="7.44140625" customWidth="1"/>
+    <col min="7" max="7" width="31" customWidth="1"/>
+    <col min="8" max="8" width="11.88671875" customWidth="1"/>
+    <col min="9" max="9" width="14.88671875" customWidth="1"/>
+    <col min="10" max="10" width="27.88671875" customWidth="1"/>
+    <col min="11" max="11" width="59.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="H3" s="22">
+        <v>45233</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="J3" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" s="15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B4" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="22">
+        <v>45233</v>
+      </c>
+      <c r="I4" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="J4" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4" s="15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B5" s="12"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="15"/>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B6" s="12"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="15"/>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B7" s="6"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="15"/>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B8" s="6"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="15"/>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B9" s="6"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="15"/>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B10" s="12"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="15"/>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B11" s="12"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="15"/>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B12" s="12"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="15"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B13" s="12"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="15"/>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B14" s="12"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="15"/>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B15" s="12"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="15"/>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B16" s="12"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="15"/>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B17" s="12"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="15"/>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B18" s="12"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="15"/>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B19" s="12"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="15"/>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B20" s="12"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="15"/>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B21" s="12"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="15"/>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B22" s="12"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="15"/>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B23" s="12"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="14"/>
+      <c r="K23" s="15"/>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B24" s="12"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="14"/>
+      <c r="K24" s="15"/>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B25" s="12"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="14"/>
+      <c r="K25" s="15"/>
+    </row>
+    <row r="26" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="16"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="18"/>
+      <c r="J26" s="18"/>
+      <c r="K26" s="19"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:K26"/>
@@ -1601,7 +2079,7 @@
   <dimension ref="B2:K26"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="B2" sqref="B2:K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2026,10 +2504,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="B2:K26"/>
+  <dimension ref="B1:K70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2046,323 +2524,324 @@
     <col min="10" max="10" width="22.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B2" s="2" t="s">
+    <row r="1" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="30" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="2:11" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="8" t="s">
+      <c r="E3" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="H3" s="9">
+      <c r="H3" s="25">
         <v>44939</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="J3" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="K3" s="10" t="s">
+      <c r="K3" s="26" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="4" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="E4" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="8" t="s">
+      <c r="E4" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="H4" s="9">
+      <c r="H4" s="31">
         <v>44939</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="I4" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="J4" s="8" t="s">
+      <c r="J4" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="K4" s="10" t="s">
+      <c r="K4" s="15" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="5" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="E5" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" s="8" t="s">
+      <c r="E5" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="H5" s="9">
+      <c r="H5" s="31">
         <v>44939</v>
       </c>
-      <c r="I5" s="8" t="s">
+      <c r="I5" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="J5" s="8" t="s">
+      <c r="J5" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="K5" s="10" t="s">
+      <c r="K5" s="15" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="E6" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="E6" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="H6" s="9">
+      <c r="H6" s="31">
         <v>44939</v>
       </c>
-      <c r="I6" s="8" t="s">
+      <c r="I6" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="J6" s="8" t="s">
+      <c r="J6" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="K6" s="10" t="s">
+      <c r="K6" s="15" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="7" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="E7" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" s="8" t="s">
+      <c r="E7" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="H7" s="9">
+      <c r="H7" s="31">
         <v>44939</v>
       </c>
-      <c r="I7" s="8" t="s">
+      <c r="I7" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="J7" s="8" t="s">
+      <c r="J7" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="K7" s="10" t="s">
+      <c r="K7" s="15" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="8" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="E8" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" s="8" t="s">
+      <c r="E8" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="H8" s="9">
+      <c r="H8" s="31">
         <v>44939</v>
       </c>
-      <c r="I8" s="8" t="s">
+      <c r="I8" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="J8" s="8" t="s">
+      <c r="J8" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="K8" s="10" t="s">
+      <c r="K8" s="15" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="9" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="E9" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G9" s="11" t="s">
+      <c r="E9" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="H9" s="9">
+      <c r="H9" s="31">
         <v>44939</v>
       </c>
-      <c r="I9" s="8" t="s">
+      <c r="I9" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="J9" s="8" t="s">
+      <c r="J9" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="K9" s="10" t="s">
+      <c r="K9" s="15" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="10" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="14" t="s">
         <v>66</v>
       </c>
       <c r="D10" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="E10" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G10" s="8" t="s">
+      <c r="E10" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="H10" s="9">
+      <c r="H10" s="31">
         <v>44939</v>
       </c>
-      <c r="I10" s="8" t="s">
+      <c r="I10" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="J10" s="8" t="s">
+      <c r="J10" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="K10" s="10" t="s">
+      <c r="K10" s="15" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="14" t="s">
         <v>68</v>
       </c>
       <c r="D11" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E11" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G11" s="8" t="s">
+      <c r="E11" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="H11" s="9">
+      <c r="H11" s="31">
         <v>44939</v>
       </c>
-      <c r="I11" s="8" t="s">
+      <c r="I11" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="J11" s="8" t="s">
+      <c r="J11" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="K11" s="10" t="s">
+      <c r="K11" s="15" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2370,7 +2849,7 @@
       <c r="B12" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="14" t="s">
         <v>99</v>
       </c>
       <c r="D12" s="14" t="s">
@@ -2385,10 +2864,10 @@
       <c r="G12" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="H12" s="23">
+      <c r="H12" s="22">
         <v>45233</v>
       </c>
-      <c r="I12" s="22" t="s">
+      <c r="I12" s="14" t="s">
         <v>105</v>
       </c>
       <c r="J12" s="14" t="s">
@@ -2402,7 +2881,7 @@
       <c r="B13" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="14" t="s">
         <v>98</v>
       </c>
       <c r="D13" s="14" t="s">
@@ -2417,7 +2896,7 @@
       <c r="G13" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="H13" s="23">
+      <c r="H13" s="22">
         <v>45233</v>
       </c>
       <c r="I13" s="14" t="s">
@@ -2434,7 +2913,7 @@
       <c r="B14" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="14" t="s">
         <v>97</v>
       </c>
       <c r="D14" s="20" t="s">
@@ -2449,7 +2928,7 @@
       <c r="G14" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="H14" s="23">
+      <c r="H14" s="22">
         <v>45233</v>
       </c>
       <c r="I14" s="14" t="s">
@@ -2466,7 +2945,7 @@
       <c r="B15" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="14" t="s">
         <v>96</v>
       </c>
       <c r="D15" s="20" t="s">
@@ -2481,7 +2960,7 @@
       <c r="G15" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="H15" s="23">
+      <c r="H15" s="22">
         <v>45233</v>
       </c>
       <c r="I15" s="14" t="s">
@@ -2498,7 +2977,7 @@
       <c r="B16" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="14" t="s">
         <v>94</v>
       </c>
       <c r="D16" s="14" t="s">
@@ -2510,10 +2989,10 @@
       <c r="F16" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="G16" s="8" t="s">
+      <c r="G16" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="H16" s="23">
+      <c r="H16" s="22">
         <v>45233</v>
       </c>
       <c r="I16" s="14" t="s">
@@ -2530,7 +3009,7 @@
       <c r="B17" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="14" t="s">
         <v>95</v>
       </c>
       <c r="D17" s="21" t="s">
@@ -2542,10 +3021,10 @@
       <c r="F17" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="G17" s="24" t="s">
+      <c r="G17" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="H17" s="23">
+      <c r="H17" s="22">
         <v>45233</v>
       </c>
       <c r="I17" s="14" t="s">
@@ -2562,7 +3041,7 @@
       <c r="B18" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="14" t="s">
         <v>110</v>
       </c>
       <c r="D18" s="14" t="s">
@@ -2574,16 +3053,16 @@
       <c r="F18" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="G18" s="8" t="s">
+      <c r="G18" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="H18" s="23">
+      <c r="H18" s="22">
         <v>45233</v>
       </c>
       <c r="I18" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="J18" s="25" t="s">
+      <c r="J18" s="14" t="s">
         <v>20</v>
       </c>
       <c r="K18" s="15" t="s">
@@ -2594,7 +3073,7 @@
       <c r="B19" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C19" s="14" t="s">
         <v>111</v>
       </c>
       <c r="D19" s="21" t="s">
@@ -2606,10 +3085,10 @@
       <c r="F19" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="G19" s="8" t="s">
+      <c r="G19" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="H19" s="23">
+      <c r="H19" s="22">
         <v>45233</v>
       </c>
       <c r="I19" s="14" t="s">
@@ -2623,32 +3102,69 @@
       </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B20" s="12"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
-      <c r="K20" s="15"/>
+      <c r="B20" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F20" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G20" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="H20" s="22">
+        <v>45233</v>
+      </c>
+      <c r="I20" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="J20" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="K20" s="15" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B21" s="12"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
-      <c r="K21" s="15"/>
+      <c r="B21" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="D21" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="E21" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F21" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H21" s="22">
+        <v>45233</v>
+      </c>
+      <c r="I21" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="J21" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="K21" s="15" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B22" s="12"/>
-      <c r="C22" s="13"/>
+      <c r="C22" s="14"/>
       <c r="D22" s="14"/>
       <c r="E22" s="14"/>
       <c r="F22" s="14"/>
@@ -2660,7 +3176,7 @@
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B23" s="12"/>
-      <c r="C23" s="13"/>
+      <c r="C23" s="14"/>
       <c r="D23" s="14"/>
       <c r="E23" s="14"/>
       <c r="F23" s="14"/>
@@ -2672,7 +3188,7 @@
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B24" s="12"/>
-      <c r="C24" s="13"/>
+      <c r="C24" s="14"/>
       <c r="D24" s="14"/>
       <c r="E24" s="14"/>
       <c r="F24" s="14"/>
@@ -2684,7 +3200,7 @@
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B25" s="12"/>
-      <c r="C25" s="13"/>
+      <c r="C25" s="14"/>
       <c r="D25" s="14"/>
       <c r="E25" s="14"/>
       <c r="F25" s="14"/>
@@ -2695,16 +3211,544 @@
       <c r="K25" s="15"/>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B26" s="16"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
-      <c r="H26" s="18"/>
-      <c r="I26" s="18"/>
-      <c r="J26" s="18"/>
-      <c r="K26" s="19"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="14"/>
+      <c r="J26" s="14"/>
+      <c r="K26" s="15"/>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B27" s="12"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="14"/>
+      <c r="I27" s="14"/>
+      <c r="J27" s="14"/>
+      <c r="K27" s="15"/>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B28" s="12"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="14"/>
+      <c r="I28" s="14"/>
+      <c r="J28" s="14"/>
+      <c r="K28" s="15"/>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B29" s="12"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="14"/>
+      <c r="J29" s="14"/>
+      <c r="K29" s="15"/>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B30" s="12"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="14"/>
+      <c r="I30" s="14"/>
+      <c r="J30" s="14"/>
+      <c r="K30" s="15"/>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B31" s="12"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="14"/>
+      <c r="I31" s="14"/>
+      <c r="J31" s="14"/>
+      <c r="K31" s="15"/>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B32" s="12"/>
+      <c r="C32" s="14"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="14"/>
+      <c r="G32" s="14"/>
+      <c r="H32" s="14"/>
+      <c r="I32" s="14"/>
+      <c r="J32" s="14"/>
+      <c r="K32" s="15"/>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B33" s="12"/>
+      <c r="C33" s="14"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="14"/>
+      <c r="G33" s="14"/>
+      <c r="H33" s="14"/>
+      <c r="I33" s="14"/>
+      <c r="J33" s="14"/>
+      <c r="K33" s="15"/>
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B34" s="12"/>
+      <c r="C34" s="14"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="14"/>
+      <c r="G34" s="14"/>
+      <c r="H34" s="14"/>
+      <c r="I34" s="14"/>
+      <c r="J34" s="14"/>
+      <c r="K34" s="15"/>
+    </row>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B35" s="12"/>
+      <c r="C35" s="14"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="14"/>
+      <c r="H35" s="14"/>
+      <c r="I35" s="14"/>
+      <c r="J35" s="14"/>
+      <c r="K35" s="15"/>
+    </row>
+    <row r="36" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B36" s="12"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="14"/>
+      <c r="G36" s="14"/>
+      <c r="H36" s="14"/>
+      <c r="I36" s="14"/>
+      <c r="J36" s="14"/>
+      <c r="K36" s="15"/>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B37" s="12"/>
+      <c r="C37" s="14"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="14"/>
+      <c r="G37" s="14"/>
+      <c r="H37" s="14"/>
+      <c r="I37" s="14"/>
+      <c r="J37" s="14"/>
+      <c r="K37" s="15"/>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B38" s="12"/>
+      <c r="C38" s="14"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="14"/>
+      <c r="G38" s="14"/>
+      <c r="H38" s="14"/>
+      <c r="I38" s="14"/>
+      <c r="J38" s="14"/>
+      <c r="K38" s="15"/>
+    </row>
+    <row r="39" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B39" s="12"/>
+      <c r="C39" s="14"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="14"/>
+      <c r="G39" s="14"/>
+      <c r="H39" s="14"/>
+      <c r="I39" s="14"/>
+      <c r="J39" s="14"/>
+      <c r="K39" s="15"/>
+    </row>
+    <row r="40" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B40" s="12"/>
+      <c r="C40" s="14"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="14"/>
+      <c r="G40" s="14"/>
+      <c r="H40" s="14"/>
+      <c r="I40" s="14"/>
+      <c r="J40" s="14"/>
+      <c r="K40" s="15"/>
+    </row>
+    <row r="41" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B41" s="12"/>
+      <c r="C41" s="14"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="14"/>
+      <c r="G41" s="14"/>
+      <c r="H41" s="14"/>
+      <c r="I41" s="14"/>
+      <c r="J41" s="14"/>
+      <c r="K41" s="15"/>
+    </row>
+    <row r="42" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B42" s="12"/>
+      <c r="C42" s="14"/>
+      <c r="D42" s="14"/>
+      <c r="E42" s="14"/>
+      <c r="F42" s="14"/>
+      <c r="G42" s="14"/>
+      <c r="H42" s="14"/>
+      <c r="I42" s="14"/>
+      <c r="J42" s="14"/>
+      <c r="K42" s="15"/>
+    </row>
+    <row r="43" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B43" s="12"/>
+      <c r="C43" s="14"/>
+      <c r="D43" s="14"/>
+      <c r="E43" s="14"/>
+      <c r="F43" s="14"/>
+      <c r="G43" s="14"/>
+      <c r="H43" s="14"/>
+      <c r="I43" s="14"/>
+      <c r="J43" s="14"/>
+      <c r="K43" s="15"/>
+    </row>
+    <row r="44" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B44" s="12"/>
+      <c r="C44" s="14"/>
+      <c r="D44" s="14"/>
+      <c r="E44" s="14"/>
+      <c r="F44" s="14"/>
+      <c r="G44" s="14"/>
+      <c r="H44" s="14"/>
+      <c r="I44" s="14"/>
+      <c r="J44" s="14"/>
+      <c r="K44" s="15"/>
+    </row>
+    <row r="45" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B45" s="12"/>
+      <c r="C45" s="14"/>
+      <c r="D45" s="14"/>
+      <c r="E45" s="14"/>
+      <c r="F45" s="14"/>
+      <c r="G45" s="14"/>
+      <c r="H45" s="14"/>
+      <c r="I45" s="14"/>
+      <c r="J45" s="14"/>
+      <c r="K45" s="15"/>
+    </row>
+    <row r="46" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B46" s="12"/>
+      <c r="C46" s="14"/>
+      <c r="D46" s="14"/>
+      <c r="E46" s="14"/>
+      <c r="F46" s="14"/>
+      <c r="G46" s="14"/>
+      <c r="H46" s="14"/>
+      <c r="I46" s="14"/>
+      <c r="J46" s="14"/>
+      <c r="K46" s="15"/>
+    </row>
+    <row r="47" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B47" s="12"/>
+      <c r="C47" s="14"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="14"/>
+      <c r="G47" s="14"/>
+      <c r="H47" s="14"/>
+      <c r="I47" s="14"/>
+      <c r="J47" s="14"/>
+      <c r="K47" s="15"/>
+    </row>
+    <row r="48" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B48" s="12"/>
+      <c r="C48" s="14"/>
+      <c r="D48" s="14"/>
+      <c r="E48" s="14"/>
+      <c r="F48" s="14"/>
+      <c r="G48" s="14"/>
+      <c r="H48" s="14"/>
+      <c r="I48" s="14"/>
+      <c r="J48" s="14"/>
+      <c r="K48" s="15"/>
+    </row>
+    <row r="49" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B49" s="12"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="14"/>
+      <c r="H49" s="14"/>
+      <c r="I49" s="14"/>
+      <c r="J49" s="14"/>
+      <c r="K49" s="15"/>
+    </row>
+    <row r="50" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B50" s="12"/>
+      <c r="C50" s="14"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="14"/>
+      <c r="G50" s="14"/>
+      <c r="H50" s="14"/>
+      <c r="I50" s="14"/>
+      <c r="J50" s="14"/>
+      <c r="K50" s="15"/>
+    </row>
+    <row r="51" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B51" s="12"/>
+      <c r="C51" s="14"/>
+      <c r="D51" s="14"/>
+      <c r="E51" s="14"/>
+      <c r="F51" s="14"/>
+      <c r="G51" s="14"/>
+      <c r="H51" s="14"/>
+      <c r="I51" s="14"/>
+      <c r="J51" s="14"/>
+      <c r="K51" s="15"/>
+    </row>
+    <row r="52" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B52" s="12"/>
+      <c r="C52" s="14"/>
+      <c r="D52" s="14"/>
+      <c r="E52" s="14"/>
+      <c r="F52" s="14"/>
+      <c r="G52" s="14"/>
+      <c r="H52" s="14"/>
+      <c r="I52" s="14"/>
+      <c r="J52" s="14"/>
+      <c r="K52" s="15"/>
+    </row>
+    <row r="53" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B53" s="12"/>
+      <c r="C53" s="14"/>
+      <c r="D53" s="14"/>
+      <c r="E53" s="14"/>
+      <c r="F53" s="14"/>
+      <c r="G53" s="14"/>
+      <c r="H53" s="14"/>
+      <c r="I53" s="14"/>
+      <c r="J53" s="14"/>
+      <c r="K53" s="15"/>
+    </row>
+    <row r="54" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B54" s="12"/>
+      <c r="C54" s="14"/>
+      <c r="D54" s="14"/>
+      <c r="E54" s="14"/>
+      <c r="F54" s="14"/>
+      <c r="G54" s="14"/>
+      <c r="H54" s="14"/>
+      <c r="I54" s="14"/>
+      <c r="J54" s="14"/>
+      <c r="K54" s="15"/>
+    </row>
+    <row r="55" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B55" s="12"/>
+      <c r="C55" s="14"/>
+      <c r="D55" s="14"/>
+      <c r="E55" s="14"/>
+      <c r="F55" s="14"/>
+      <c r="G55" s="14"/>
+      <c r="H55" s="14"/>
+      <c r="I55" s="14"/>
+      <c r="J55" s="14"/>
+      <c r="K55" s="15"/>
+    </row>
+    <row r="56" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B56" s="12"/>
+      <c r="C56" s="14"/>
+      <c r="D56" s="14"/>
+      <c r="E56" s="14"/>
+      <c r="F56" s="14"/>
+      <c r="G56" s="14"/>
+      <c r="H56" s="14"/>
+      <c r="I56" s="14"/>
+      <c r="J56" s="14"/>
+      <c r="K56" s="15"/>
+    </row>
+    <row r="57" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B57" s="12"/>
+      <c r="C57" s="14"/>
+      <c r="D57" s="14"/>
+      <c r="E57" s="14"/>
+      <c r="F57" s="14"/>
+      <c r="G57" s="14"/>
+      <c r="H57" s="14"/>
+      <c r="I57" s="14"/>
+      <c r="J57" s="14"/>
+      <c r="K57" s="15"/>
+    </row>
+    <row r="58" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B58" s="12"/>
+      <c r="C58" s="14"/>
+      <c r="D58" s="14"/>
+      <c r="E58" s="14"/>
+      <c r="F58" s="14"/>
+      <c r="G58" s="14"/>
+      <c r="H58" s="14"/>
+      <c r="I58" s="14"/>
+      <c r="J58" s="14"/>
+      <c r="K58" s="15"/>
+    </row>
+    <row r="59" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B59" s="12"/>
+      <c r="C59" s="14"/>
+      <c r="D59" s="14"/>
+      <c r="E59" s="14"/>
+      <c r="F59" s="14"/>
+      <c r="G59" s="14"/>
+      <c r="H59" s="14"/>
+      <c r="I59" s="14"/>
+      <c r="J59" s="14"/>
+      <c r="K59" s="15"/>
+    </row>
+    <row r="60" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B60" s="12"/>
+      <c r="C60" s="14"/>
+      <c r="D60" s="14"/>
+      <c r="E60" s="14"/>
+      <c r="F60" s="14"/>
+      <c r="G60" s="14"/>
+      <c r="H60" s="14"/>
+      <c r="I60" s="14"/>
+      <c r="J60" s="14"/>
+      <c r="K60" s="15"/>
+    </row>
+    <row r="61" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B61" s="12"/>
+      <c r="C61" s="14"/>
+      <c r="D61" s="14"/>
+      <c r="E61" s="14"/>
+      <c r="F61" s="14"/>
+      <c r="G61" s="14"/>
+      <c r="H61" s="14"/>
+      <c r="I61" s="14"/>
+      <c r="J61" s="14"/>
+      <c r="K61" s="15"/>
+    </row>
+    <row r="62" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B62" s="12"/>
+      <c r="C62" s="14"/>
+      <c r="D62" s="14"/>
+      <c r="E62" s="14"/>
+      <c r="F62" s="14"/>
+      <c r="G62" s="14"/>
+      <c r="H62" s="14"/>
+      <c r="I62" s="14"/>
+      <c r="J62" s="14"/>
+      <c r="K62" s="15"/>
+    </row>
+    <row r="63" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B63" s="12"/>
+      <c r="C63" s="14"/>
+      <c r="D63" s="14"/>
+      <c r="E63" s="14"/>
+      <c r="F63" s="14"/>
+      <c r="G63" s="14"/>
+      <c r="H63" s="14"/>
+      <c r="I63" s="14"/>
+      <c r="J63" s="14"/>
+      <c r="K63" s="15"/>
+    </row>
+    <row r="64" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B64" s="12"/>
+      <c r="C64" s="14"/>
+      <c r="D64" s="14"/>
+      <c r="E64" s="14"/>
+      <c r="F64" s="14"/>
+      <c r="G64" s="14"/>
+      <c r="H64" s="14"/>
+      <c r="I64" s="14"/>
+      <c r="J64" s="14"/>
+      <c r="K64" s="15"/>
+    </row>
+    <row r="65" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B65" s="12"/>
+      <c r="C65" s="14"/>
+      <c r="D65" s="14"/>
+      <c r="E65" s="14"/>
+      <c r="F65" s="14"/>
+      <c r="G65" s="14"/>
+      <c r="H65" s="14"/>
+      <c r="I65" s="14"/>
+      <c r="J65" s="14"/>
+      <c r="K65" s="15"/>
+    </row>
+    <row r="66" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B66" s="12"/>
+      <c r="C66" s="14"/>
+      <c r="D66" s="14"/>
+      <c r="E66" s="14"/>
+      <c r="F66" s="14"/>
+      <c r="G66" s="14"/>
+      <c r="H66" s="14"/>
+      <c r="I66" s="14"/>
+      <c r="J66" s="14"/>
+      <c r="K66" s="15"/>
+    </row>
+    <row r="67" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B67" s="12"/>
+      <c r="C67" s="14"/>
+      <c r="D67" s="14"/>
+      <c r="E67" s="14"/>
+      <c r="F67" s="14"/>
+      <c r="G67" s="14"/>
+      <c r="H67" s="14"/>
+      <c r="I67" s="14"/>
+      <c r="J67" s="14"/>
+      <c r="K67" s="15"/>
+    </row>
+    <row r="68" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B68" s="12"/>
+      <c r="C68" s="14"/>
+      <c r="D68" s="14"/>
+      <c r="E68" s="14"/>
+      <c r="F68" s="14"/>
+      <c r="G68" s="14"/>
+      <c r="H68" s="14"/>
+      <c r="I68" s="14"/>
+      <c r="J68" s="14"/>
+      <c r="K68" s="15"/>
+    </row>
+    <row r="69" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B69" s="12"/>
+      <c r="C69" s="14"/>
+      <c r="D69" s="14"/>
+      <c r="E69" s="14"/>
+      <c r="F69" s="14"/>
+      <c r="G69" s="14"/>
+      <c r="H69" s="14"/>
+      <c r="I69" s="14"/>
+      <c r="J69" s="14"/>
+      <c r="K69" s="15"/>
+    </row>
+    <row r="70" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B70" s="16"/>
+      <c r="C70" s="18"/>
+      <c r="D70" s="18"/>
+      <c r="E70" s="18"/>
+      <c r="F70" s="18"/>
+      <c r="G70" s="18"/>
+      <c r="H70" s="18"/>
+      <c r="I70" s="18"/>
+      <c r="J70" s="18"/>
+      <c r="K70" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -3357,13 +4401,1207 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8384E001-6848-4DF9-887A-D16CBA3B1E8F}">
+  <dimension ref="B1:K26"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="21.5546875" customWidth="1"/>
+    <col min="3" max="3" width="19.77734375" customWidth="1"/>
+    <col min="4" max="4" width="23.88671875" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" customWidth="1"/>
+    <col min="6" max="6" width="7.44140625" customWidth="1"/>
+    <col min="7" max="7" width="31" customWidth="1"/>
+    <col min="8" max="8" width="11.88671875" customWidth="1"/>
+    <col min="9" max="9" width="14.88671875" customWidth="1"/>
+    <col min="10" max="10" width="27.88671875" customWidth="1"/>
+    <col min="11" max="11" width="59.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="H3" s="22">
+        <v>45233</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="J3" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" s="15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B4" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="H4" s="22">
+        <v>45233</v>
+      </c>
+      <c r="I4" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="J4" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4" s="15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B5" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="H5" s="22">
+        <v>45233</v>
+      </c>
+      <c r="I5" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="J5" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5" s="15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B6" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="H6" s="22">
+        <v>45233</v>
+      </c>
+      <c r="I6" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="J6" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="K6" s="15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B7" s="6"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="15"/>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B8" s="6"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="15"/>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B9" s="6"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="15"/>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B10" s="12"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="15"/>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B11" s="12"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="15"/>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B12" s="12"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="15"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B13" s="12"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="15"/>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B14" s="12"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="15"/>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B15" s="12"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="15"/>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B16" s="12"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="15"/>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B17" s="12"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="15"/>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B18" s="12"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="15"/>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B19" s="12"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="15"/>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B20" s="12"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="15"/>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B21" s="12"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="15"/>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B22" s="12"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="15"/>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B23" s="12"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="14"/>
+      <c r="K23" s="15"/>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B24" s="12"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="14"/>
+      <c r="K24" s="15"/>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B25" s="12"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="14"/>
+      <c r="K25" s="15"/>
+    </row>
+    <row r="26" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="16"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="18"/>
+      <c r="J26" s="18"/>
+      <c r="K26" s="19"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{106023BC-FDF3-4744-A32A-62228143CA41}">
+  <dimension ref="B1:K26"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="21.5546875" customWidth="1"/>
+    <col min="3" max="3" width="19.77734375" customWidth="1"/>
+    <col min="4" max="4" width="23.88671875" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" customWidth="1"/>
+    <col min="6" max="6" width="7.44140625" customWidth="1"/>
+    <col min="7" max="7" width="31" customWidth="1"/>
+    <col min="8" max="8" width="11.88671875" customWidth="1"/>
+    <col min="9" max="9" width="14.88671875" customWidth="1"/>
+    <col min="10" max="10" width="27.88671875" customWidth="1"/>
+    <col min="11" max="11" width="59.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="H3" s="22">
+        <v>45233</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="J3" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" s="15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B4" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="H4" s="22">
+        <v>45233</v>
+      </c>
+      <c r="I4" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="J4" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4" s="15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B5" s="12"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="15"/>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B6" s="12"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="15"/>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B7" s="6"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="15"/>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B8" s="6"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="15"/>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B9" s="6"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="15"/>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B10" s="12"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="15"/>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B11" s="12"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="15"/>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B12" s="12"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="15"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B13" s="12"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="15"/>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B14" s="12"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="15"/>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B15" s="12"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="15"/>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B16" s="12"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="15"/>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B17" s="12"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="15"/>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B18" s="12"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="15"/>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B19" s="12"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="15"/>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B20" s="12"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="15"/>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B21" s="12"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="15"/>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B22" s="12"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="15"/>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B23" s="12"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="14"/>
+      <c r="K23" s="15"/>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B24" s="12"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="14"/>
+      <c r="K24" s="15"/>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B25" s="12"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="14"/>
+      <c r="K25" s="15"/>
+    </row>
+    <row r="26" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="16"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="18"/>
+      <c r="J26" s="18"/>
+      <c r="K26" s="19"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD36BE9A-A355-4C8E-A6ED-3AF4AE1439F6}">
+  <dimension ref="B1:K26"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="21.5546875" customWidth="1"/>
+    <col min="3" max="3" width="19.77734375" customWidth="1"/>
+    <col min="4" max="4" width="23.88671875" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" customWidth="1"/>
+    <col min="6" max="6" width="7.44140625" customWidth="1"/>
+    <col min="7" max="7" width="31" customWidth="1"/>
+    <col min="8" max="8" width="11.88671875" customWidth="1"/>
+    <col min="9" max="9" width="14.88671875" customWidth="1"/>
+    <col min="10" max="10" width="27.88671875" customWidth="1"/>
+    <col min="11" max="11" width="59.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="H3" s="22">
+        <v>45233</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="J3" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" s="15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B4" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="H4" s="22">
+        <v>45233</v>
+      </c>
+      <c r="I4" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="J4" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4" s="15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B5" s="12"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="15"/>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B6" s="12"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="15"/>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B7" s="6"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="15"/>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B8" s="6"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="15"/>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B9" s="6"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="15"/>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B10" s="12"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="15"/>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B11" s="12"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="15"/>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B12" s="12"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="15"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B13" s="12"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="15"/>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B14" s="12"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="15"/>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B15" s="12"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="15"/>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B16" s="12"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="15"/>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B17" s="12"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="15"/>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B18" s="12"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="15"/>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B19" s="12"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="15"/>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B20" s="12"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="15"/>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B21" s="12"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="15"/>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B22" s="12"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="15"/>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B23" s="12"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="14"/>
+      <c r="K23" s="15"/>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B24" s="12"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="14"/>
+      <c r="K24" s="15"/>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B25" s="12"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="14"/>
+      <c r="K25" s="15"/>
+    </row>
+    <row r="26" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="16"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="18"/>
+      <c r="J26" s="18"/>
+      <c r="K26" s="19"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>

</xml_diff>